<commit_message>
Updated scraped data based on links.py change
</commit_message>
<xml_diff>
--- a/Engaged_College_Financial_Metrics.xlsx
+++ b/Engaged_College_Financial_Metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -680,62 +680,62 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>UTICA UNIVERSITY</t>
+          <t>LEE UNIVERSITY</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://projects.propublica.org/nonprofits/organizations/161476258/202401069349301215/full</t>
+          <t>https://projects.propublica.org/nonprofits/organizations/620502739/202401319349302970/full</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>89,786,192</t>
+          <t>97,254,831</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>105,142,781</t>
+          <t>108,753,431</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>105,687,698</t>
+          <t>93,462,606</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>104,853,806</t>
+          <t>105,914,787</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>56,835,779</t>
+          <t>166,167,918</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>74,318,287</t>
+          <t>160,791,459</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2,294</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>5,256,315</t>
+          <t>10,985,421</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>30,921,523</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>4,309,285</t>
+          <t>30,946,403</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -745,27 +745,27 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>40,489,417</t>
+          <t>41,931,824</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>7,150</t>
+          <t>0</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>16,579,558</t>
+          <t>6,600,350</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>28,864,607</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>6,835,827</t>
+          <t>32,018,540</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -775,147 +775,25 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>52,287,142</t>
+          <t>38,618,890</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>-17.71</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>0.27</t>
+          <t>2.61</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>38.31</t>
+          <t>44.86</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
-        <is>
-          <t>49.87</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>LEE UNIVERSITY</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://projects.propublica.org/nonprofits/organizations/620502739/202401319349302970/full</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>97,254,831</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>108,753,431</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>93,462,606</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>105,914,787</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>166,167,918</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>160,791,459</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>10,985,421</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>30,946,403</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>41,931,824</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>6,600,350</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>32,018,540</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>38,618,890</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>3.9</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>2.61</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>44.86</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
         <is>
           <t>36.46</t>
         </is>

</xml_diff>